<commit_message>
Added convertFitness method to CsvResultConverter
</commit_message>
<xml_diff>
--- a/wykresy/f(x)=2 ln(x+1).xlsx
+++ b/wykresy/f(x)=2 ln(x+1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Studia\5 sem\Programowanie genetyczne\tiny-gp\wykresy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354F246F-74D7-4EEB-918F-A0A8A18DDAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719AA3A5-891A-4FF7-81E5-03BCF53E18B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(0,4)" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>x1</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>program result</t>
+  </si>
+  <si>
+    <t>generation</t>
+  </si>
+  <si>
+    <t>bestFitness</t>
+  </si>
+  <si>
+    <t>averageFitness</t>
   </si>
 </sst>
 </file>
@@ -2758,304 +2767,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.19405367023805201</c:v>
+                  <c:v>-4.8185726708956499E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.339898517693138</c:v>
+                  <c:v>0.168719904195613</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47612557332168898</c:v>
+                  <c:v>0.33147420448043002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60391226948591803</c:v>
+                  <c:v>0.48356032212375699</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72427782189470902</c:v>
+                  <c:v>0.62540113815960896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83806488195620898</c:v>
+                  <c:v>0.75763920092259096</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94598154114374799</c:v>
+                  <c:v>0.88104881552637704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0486280830210799</c:v>
+                  <c:v>0.99646019237380501</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.14651726949343</c:v>
+                  <c:v>1.10470149512032</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2400901413885199</c:v>
+                  <c:v>1.2065593974142099</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3297284841114501</c:v>
+                  <c:v>1.30275570143469</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4157647598617999</c:v>
+                  <c:v>1.39393634010724</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.49849009031364</c:v>
+                  <c:v>1.48066904137813</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.57816072353073</c:v>
+                  <c:v>1.56344649175098</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.65500331158444</c:v>
+                  <c:v>1.6426925910877399</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.7292192472157299</c:v>
+                  <c:v>1.7187701137376299</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8009882502475401</c:v>
+                  <c:v>1.7919886842207799</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8704713514695399</c:v>
+                  <c:v>1.86261241749457</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9378133893442899</c:v>
+                  <c:v>1.93086687998377</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0031451102864999</c:v>
+                  <c:v>1.99694522676479</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.06658494441993</c:v>
+                  <c:v>2.0610134917832901</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1282405141646299</c:v>
+                  <c:v>2.1232150763139299</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1882099216882498</c:v>
+                  <c:v>2.1836745146825201</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2465828523901501</c:v>
+                  <c:v>2.2425006087980002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.30344152459935</c:v>
+                  <c:v>2.29978902321393</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3588615101239401</c:v>
+                  <c:v>2.3556244260314601</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4129124458675202</c:v>
+                  <c:v>2.4100822515461999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4656586531798199</c:v>
+                  <c:v>2.4632301502463001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.5171596787470198</c:v>
+                  <c:v>2.5151291817623802</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5674707685068299</c:v>
+                  <c:v>2.5658347972418398</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.61664328418416</c:v>
+                  <c:v>2.6153976496093199</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.6647250704959302</c:v>
+                  <c:v>2.6638642633226901</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.7117607798029</c:v>
+                  <c:v>2.7112775894740602</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.7577921599366602</c:v>
+                  <c:v>2.7576774673033602</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.8028583100604201</c:v>
+                  <c:v>2.8031010092570399</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.8469959086985699</c:v>
+                  <c:v>2.8475829235065202</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.8902394511536902</c:v>
+                  <c:v>2.89115578522195</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.9326212985389799</c:v>
+                  <c:v>2.93385026577034</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.9741720397290199</c:v>
+                  <c:v>2.9756953272858002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.0149205078523398</c:v>
+                  <c:v>3.0167183886662001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.0548939062376901</c:v>
+                  <c:v>3.0569454679245398</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.0941180840304998</c:v>
+                  <c:v>3.09640130491234</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.13261741362225</c:v>
+                  <c:v>3.13510946769577</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.17041504185765</c:v>
+                  <c:v>3.17309244526886</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.2075329417465599</c:v>
+                  <c:v>3.2103717288048301</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.2439919939635198</c:v>
+                  <c:v>3.2469678832543898</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.2798120611694701</c:v>
+                  <c:v>3.2829006107813599</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.3150120559033698</c:v>
+                  <c:v>3.3181888072664401</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.3496100027028399</c:v>
+                  <c:v>3.3528506128986999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.3836230950364001</c:v>
+                  <c:v>3.3869034577016102</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.4170677475639901</c:v>
+                  <c:v>3.42036410269897</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.4499596441862801</c:v>
+                  <c:v>3.4532486773103099</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.48231378229648</c:v>
+                  <c:v>3.4855727134699701</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.5141445136127798</c:v>
+                  <c:v>3.5173511768856098</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.5454655819511198</c:v>
+                  <c:v>3.5485984957870702</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.5762901583148601</c:v>
+                  <c:v>3.5793285874628</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.6066308737891499</c:v>
+                  <c:v>3.6095548828367701</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.6364998511558899</c:v>
+                  <c:v>3.6392903493014699</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.6659087379020798</c:v>
+                  <c:v>3.6685475119919202</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.69486875274885</c:v>
+                  <c:v>3.69733847365982</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.7233908460263301</c:v>
+                  <c:v>3.7256749332851</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.75149572672274</c:v>
+                  <c:v>3.75356820354409</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.7791584246191099</c:v>
+                  <c:v>3.7810292272381498</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.80642643116418</c:v>
+                  <c:v>3.80806859277356</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.8332948728413698</c:v>
+                  <c:v>3.8346965487723099</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.8597729189286198</c:v>
+                  <c:v>3.8609230178843701</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.8858691739590299</c:v>
+                  <c:v>3.8867576098635599</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.9115918975339201</c:v>
+                  <c:v>3.91220963396258</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>3.9369490452361302</c:v>
+                  <c:v>3.9372881106967301</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.9619482880564498</c:v>
+                  <c:v>3.96200178302059</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.9865970265755801</c:v>
+                  <c:v>3.9863591269578298</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.0109024030858498</c:v>
+                  <c:v>4.0103683617200998</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.0348713125397104</c:v>
+                  <c:v>4.0340374593478296</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.0585104126464397</c:v>
+                  <c:v>4.0573741539027299</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.08182613326428</c:v>
+                  <c:v>4.08038595023912</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.1048246851713097</c:v>
+                  <c:v>4.1030801323792199</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.1275120682709998</c:v>
+                  <c:v>4.1254637715149798</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.1498940792749401</c:v>
+                  <c:v>4.1475437336578196</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.17197631889759</c:v>
+                  <c:v>4.1693266869555803</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4.1937641985925502</c:v>
+                  <c:v>4.1908191086947797</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.2152629468563703</c:v>
+                  <c:v>4.21202729200491</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.2364776151227597</c:v>
+                  <c:v>4.2329573522802901</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.2574130832677302</c:v>
+                  <c:v>4.2536152333341199</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.2780740647437199</c:v>
+                  <c:v>4.2740067132980304</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.29846511135894</c:v>
+                  <c:v>4.2941374102801202</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.3185906177162501</c:v>
+                  <c:v>4.3140127877930601</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.3384548253241499</c:v>
+                  <c:v>4.3336381599635798</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.3580618263907898</c:v>
+                  <c:v>4.3530186965337601</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.3774155673103303</c:v>
+                  <c:v>4.3721594276639504</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.3965198518496198</c:v>
+                  <c:v>4.3910652485466501</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.4153783440413603</c:v>
+                  <c:v>4.4097409238400296</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>4.43399457078878</c:v>
+                  <c:v>4.4281910919294001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.45237192418523</c:v>
+                  <c:v>4.4464202690244896</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.4705136635506699</c:v>
+                  <c:v>4.4644328530997504</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.4884229171855603</c:v>
+                  <c:v>4.4822331276848804</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.5061026838412097</c:v>
+                  <c:v>4.4998252655120297</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4.5235558339039201</c:v>
+                  <c:v>4.5172133320260501</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>4.5407851102889003</c:v>
+                  <c:v>4.5344012887637497</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>4.5577931290379397</c:v>
+                  <c:v>4.5513929966077598</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.5745823796132603</c:v>
+                  <c:v>4.5681922189203501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3300,6 +3309,978 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'(0,9)'!$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bestFitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'(0,9)'!$X$2:$X$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'(0,9)'!$Y$2:$Y$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>26.738412923971001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0631597346656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.0631597346656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.0631597346656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.2497718786462</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.799082899456099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4082040258236201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2487260549043597</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2487260549043597</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2487260549043597</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2487260549043597</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.9192287194321898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.7303051084612902</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3380703737813699</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3035415315442802</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7520066398893599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.72330112149083</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.72330112149083</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4334885533441599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4334885533441599</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.26738144157502</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9774894719487299</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.9774894719487299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.85278035444737</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.8525510990571801</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7356988167376599</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4139862932214899</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3860775093170301</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3859521313788901</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3859521313788901</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3603191049577199</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.25548750131307</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.81246801191321905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4858-409B-9182-DEC92B7FBC77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1225880592"/>
+        <c:axId val="1059749632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1225880592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1059749632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1059749632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1225880592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'(0,9)'!$Z$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>averageFitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'(0,9)'!$X$2:$X$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'(0,9)'!$Z$2:$Z$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>5018.6356083259698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>923.98394371503798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>406.72304032442997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>296.69820480887802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>291.32531189932098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>281.68560823021699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360.37463320169701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>403.03715264152999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>342.73314466248502</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304.02453756897</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>308.80557700156902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>296.88314172881798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>306.33650622076902</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>192.69431516230301</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>205.018481074823</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>204.15653813771701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>249.875487520902</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>267.85143922622001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>268.60278037953901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>325.82245778669699</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>281.89087953238601</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>227.93202545527299</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>189.17118372503401</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>171.88966729656801</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1449.7506534121601</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>227.68338080988099</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>291.16034211988199</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>343.59560671276199</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>484.47142513326298</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>208.301894686427</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>628.60645221346203</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>374.441507775856</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4230.3187759682496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B138-4311-B17F-22C5054A05FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1225874832"/>
+        <c:axId val="1059763520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1225874832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1059763520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1059763520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1225874832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -4882,7 +5863,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
@@ -6639,6 +7620,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8188,6 +9249,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8748,16 +10841,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8777,6 +10870,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89E88F7C-5757-30F7-BD28-790BC94B48CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{718B2E7C-5B11-8DBB-4443-2D7B3EDB0C37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9132,7 +11297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
@@ -10257,15 +12422,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED20EBBC-6679-46F5-867A-81C8CA9C8BC4}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10275,8 +12440,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10284,10 +12458,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.19405367023805201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-4.8185726708956499E-3</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>26.738412923971001</v>
+      </c>
+      <c r="Z2">
+        <v>5018.6356083259698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.09</v>
       </c>
@@ -10295,10 +12478,19 @@
         <v>0.17235539248210399</v>
       </c>
       <c r="C3">
-        <v>0.339898517693138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.168719904195613</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>24.0631597346656</v>
+      </c>
+      <c r="Z3">
+        <v>923.98394371503798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.18</v>
       </c>
@@ -10306,10 +12498,19 @@
         <v>0.33102887695514599</v>
       </c>
       <c r="C4">
-        <v>0.47612557332168898</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.33147420448043002</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="Y4">
+        <v>24.0631597346656</v>
+      </c>
+      <c r="Z4">
+        <v>406.72304032442997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.27</v>
       </c>
@@ -10317,10 +12518,19 @@
         <v>0.47803380094099901</v>
       </c>
       <c r="C5">
-        <v>0.60391226948591803</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.48356032212375699</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+      <c r="Y5">
+        <v>24.0631597346656</v>
+      </c>
+      <c r="Z5">
+        <v>296.69820480887802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.36</v>
       </c>
@@ -10328,10 +12538,19 @@
         <v>0.614969399495921</v>
       </c>
       <c r="C6">
-        <v>0.72427782189470902</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.62540113815960896</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
+      <c r="Y6">
+        <v>23.2497718786462</v>
+      </c>
+      <c r="Z6">
+        <v>291.32531189932098</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.44999999999999901</v>
       </c>
@@ -10339,10 +12558,19 @@
         <v>0.74312711286496602</v>
       </c>
       <c r="C7">
-        <v>0.83806488195620898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75763920092259096</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+      <c r="Y7">
+        <v>10.799082899456099</v>
+      </c>
+      <c r="Z7">
+        <v>281.68560823021699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.53999999999999904</v>
       </c>
@@ -10350,10 +12578,19 @@
         <v>0.86356483285107499</v>
       </c>
       <c r="C8">
-        <v>0.94598154114374799</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88104881552637704</v>
+      </c>
+      <c r="X8">
+        <v>7</v>
+      </c>
+      <c r="Y8">
+        <v>8.4082040258236201</v>
+      </c>
+      <c r="Z8">
+        <v>360.37463320169701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.62999999999999901</v>
       </c>
@@ -10361,10 +12598,19 @@
         <v>0.97716002963734105</v>
       </c>
       <c r="C9">
-        <v>1.0486280830210799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.99646019237380501</v>
+      </c>
+      <c r="X9">
+        <v>8</v>
+      </c>
+      <c r="Y9">
+        <v>6.2487260549043597</v>
+      </c>
+      <c r="Z9">
+        <v>403.03715264152999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.71999999999999897</v>
       </c>
@@ -10372,10 +12618,19 @@
         <v>1.0846485816507201</v>
       </c>
       <c r="C10">
-        <v>1.14651726949343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.10470149512032</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
+      <c r="Y10">
+        <v>6.2487260549043597</v>
+      </c>
+      <c r="Z10">
+        <v>342.73314466248502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.80999999999999905</v>
       </c>
@@ -10383,10 +12638,19 @@
         <v>1.1866536905554601</v>
       </c>
       <c r="C11">
-        <v>1.2400901413885199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.2065593974142099</v>
+      </c>
+      <c r="X11">
+        <v>10</v>
+      </c>
+      <c r="Y11">
+        <v>6.2487260549043597</v>
+      </c>
+      <c r="Z11">
+        <v>304.02453756897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.89999999999999902</v>
       </c>
@@ -10394,10 +12658,19 @@
         <v>1.2837077723447801</v>
       </c>
       <c r="C12">
-        <v>1.3297284841114501</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.30275570143469</v>
+      </c>
+      <c r="X12">
+        <v>11</v>
+      </c>
+      <c r="Y12">
+        <v>6.2487260549043597</v>
+      </c>
+      <c r="Z12">
+        <v>308.80557700156902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.98999999999999899</v>
       </c>
@@ -10405,10 +12678,19 @@
         <v>1.3762692774728</v>
       </c>
       <c r="C13">
-        <v>1.4157647598617999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.39393634010724</v>
+      </c>
+      <c r="X13">
+        <v>12</v>
+      </c>
+      <c r="Y13">
+        <v>5.9192287194321898</v>
+      </c>
+      <c r="Z13">
+        <v>296.88314172881798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.0799999999999901</v>
       </c>
@@ -10416,10 +12698,19 @@
         <v>1.4647357874264499</v>
       </c>
       <c r="C14">
-        <v>1.49849009031364</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.48066904137813</v>
+      </c>
+      <c r="X14">
+        <v>13</v>
+      </c>
+      <c r="Y14">
+        <v>3.7303051084612902</v>
+      </c>
+      <c r="Z14">
+        <v>306.33650622076902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.17</v>
       </c>
@@ -10427,10 +12718,19 @@
         <v>1.5494543351047301</v>
       </c>
       <c r="C15">
-        <v>1.57816072353073</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.56344649175098</v>
+      </c>
+      <c r="X15">
+        <v>14</v>
+      </c>
+      <c r="Y15">
+        <v>3.3380703737813699</v>
+      </c>
+      <c r="Z15">
+        <v>192.69431516230301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.26</v>
       </c>
@@ -10438,10 +12738,19 @@
         <v>1.6307296265683799</v>
       </c>
       <c r="C16">
-        <v>1.65500331158444</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.6426925910877399</v>
+      </c>
+      <c r="X16">
+        <v>15</v>
+      </c>
+      <c r="Y16">
+        <v>3.3035415315442802</v>
+      </c>
+      <c r="Z16">
+        <v>205.018481074823</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.35</v>
       </c>
@@ -10449,10 +12758,19 @@
         <v>1.70883065631213</v>
       </c>
       <c r="C17">
-        <v>1.7292192472157299</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.7187701137376299</v>
+      </c>
+      <c r="X17">
+        <v>16</v>
+      </c>
+      <c r="Y17">
+        <v>2.7520066398893599</v>
+      </c>
+      <c r="Z17">
+        <v>204.15653813771701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.44</v>
       </c>
@@ -10460,10 +12778,19 @@
         <v>1.78399607861022</v>
       </c>
       <c r="C18">
-        <v>1.8009882502475401</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.7919886842207799</v>
+      </c>
+      <c r="X18">
+        <v>17</v>
+      </c>
+      <c r="Y18">
+        <v>2.72330112149083</v>
+      </c>
+      <c r="Z18">
+        <v>249.875487520902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.53</v>
       </c>
@@ -10471,10 +12798,19 @@
         <v>1.85643860547885</v>
       </c>
       <c r="C19">
-        <v>1.8704713514695399</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.86261241749457</v>
+      </c>
+      <c r="X19">
+        <v>18</v>
+      </c>
+      <c r="Y19">
+        <v>2.72330112149083</v>
+      </c>
+      <c r="Z19">
+        <v>267.85143922622001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.62</v>
       </c>
@@ -10482,10 +12818,19 @@
         <v>1.92634863554601</v>
       </c>
       <c r="C20">
-        <v>1.9378133893442899</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.93086687998377</v>
+      </c>
+      <c r="X20">
+        <v>19</v>
+      </c>
+      <c r="Y20">
+        <v>2.4334885533441599</v>
+      </c>
+      <c r="Z20">
+        <v>268.60278037953901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.71</v>
       </c>
@@ -10493,10 +12838,19 @@
         <v>1.99389726978321</v>
       </c>
       <c r="C21">
-        <v>2.0031451102864999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.99694522676479</v>
+      </c>
+      <c r="X21">
+        <v>20</v>
+      </c>
+      <c r="Y21">
+        <v>2.4334885533441599</v>
+      </c>
+      <c r="Z21">
+        <v>325.82245778669699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.8</v>
       </c>
@@ -10504,10 +12858,19 @@
         <v>2.05923883436231</v>
       </c>
       <c r="C22">
-        <v>2.06658494441993</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0610134917832901</v>
+      </c>
+      <c r="X22">
+        <v>21</v>
+      </c>
+      <c r="Y22">
+        <v>2.26738144157502</v>
+      </c>
+      <c r="Z22">
+        <v>281.89087953238601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.89</v>
       </c>
@@ -10515,10 +12878,19 @@
         <v>2.1225130042486802</v>
       </c>
       <c r="C23">
-        <v>2.1282405141646299</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.1232150763139299</v>
+      </c>
+      <c r="X23">
+        <v>22</v>
+      </c>
+      <c r="Y23">
+        <v>1.9774894719487299</v>
+      </c>
+      <c r="Z23">
+        <v>227.93202545527299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.98</v>
       </c>
@@ -10526,10 +12898,19 @@
         <v>2.1838466010346198</v>
       </c>
       <c r="C24">
-        <v>2.1882099216882498</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.1836745146825201</v>
+      </c>
+      <c r="X24">
+        <v>23</v>
+      </c>
+      <c r="Y24">
+        <v>1.9774894719487299</v>
+      </c>
+      <c r="Z24">
+        <v>189.17118372503401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2.0699999999999998</v>
       </c>
@@ -10537,10 +12918,19 @@
         <v>2.2433551231982101</v>
       </c>
       <c r="C25">
-        <v>2.2465828523901501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.2425006087980002</v>
+      </c>
+      <c r="X25">
+        <v>24</v>
+      </c>
+      <c r="Y25">
+        <v>1.85278035444737</v>
+      </c>
+      <c r="Z25">
+        <v>171.88966729656801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2.16</v>
       </c>
@@ -10548,10 +12938,19 @@
         <v>2.3011440551976401</v>
       </c>
       <c r="C26">
-        <v>2.30344152459935</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.29978902321393</v>
+      </c>
+      <c r="X26">
+        <v>25</v>
+      </c>
+      <c r="Y26">
+        <v>1.8525510990571801</v>
+      </c>
+      <c r="Z26">
+        <v>1449.7506534121601</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2.25</v>
       </c>
@@ -10559,10 +12958,19 @@
         <v>2.3573099926832901</v>
       </c>
       <c r="C27">
-        <v>2.3588615101239401</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.3556244260314601</v>
+      </c>
+      <c r="X27">
+        <v>26</v>
+      </c>
+      <c r="Y27">
+        <v>1.7356988167376599</v>
+      </c>
+      <c r="Z27">
+        <v>227.68338080988099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2.34</v>
       </c>
@@ -10570,10 +12978,19 @@
         <v>2.4119416139772101</v>
       </c>
       <c r="C28">
-        <v>2.4129124458675202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4100822515461999</v>
+      </c>
+      <c r="X28">
+        <v>27</v>
+      </c>
+      <c r="Y28">
+        <v>1.4139862932214899</v>
+      </c>
+      <c r="Z28">
+        <v>291.16034211988199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2.4300000000000002</v>
       </c>
@@ -10581,10 +12998,19 @@
         <v>2.46512052235569</v>
       </c>
       <c r="C29">
-        <v>2.4656586531798199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4632301502463001</v>
+      </c>
+      <c r="X29">
+        <v>28</v>
+      </c>
+      <c r="Y29">
+        <v>1.3860775093170301</v>
+      </c>
+      <c r="Z29">
+        <v>343.59560671276199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2.52</v>
       </c>
@@ -10592,10 +13018,19 @@
         <v>2.5169219792200099</v>
       </c>
       <c r="C30">
-        <v>2.5171596787470198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.5151291817623802</v>
+      </c>
+      <c r="X30">
+        <v>29</v>
+      </c>
+      <c r="Y30">
+        <v>1.3859521313788901</v>
+      </c>
+      <c r="Z30">
+        <v>484.47142513326298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2.61</v>
       </c>
@@ -10603,10 +13038,19 @@
         <v>2.5674155446895699</v>
       </c>
       <c r="C31">
-        <v>2.5674707685068299</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.5658347972418398</v>
+      </c>
+      <c r="X31">
+        <v>30</v>
+      </c>
+      <c r="Y31">
+        <v>1.3859521313788901</v>
+      </c>
+      <c r="Z31">
+        <v>208.301894686427</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2.69999999999999</v>
       </c>
@@ -10614,10 +13058,19 @@
         <v>2.6166656393003498</v>
       </c>
       <c r="C32">
-        <v>2.61664328418416</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.6153976496093199</v>
+      </c>
+      <c r="X32">
+        <v>31</v>
+      </c>
+      <c r="Y32">
+        <v>1.3603191049577199</v>
+      </c>
+      <c r="Z32">
+        <v>628.60645221346203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2.7899999999999898</v>
       </c>
@@ -10625,10 +13078,19 @@
         <v>2.6647320381886699</v>
       </c>
       <c r="C33">
-        <v>2.6647250704959302</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.6638642633226901</v>
+      </c>
+      <c r="X33">
+        <v>32</v>
+      </c>
+      <c r="Y33">
+        <v>1.25548750131307</v>
+      </c>
+      <c r="Z33">
+        <v>374.441507775856</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2.8799999999999901</v>
       </c>
@@ -10636,10 +13098,19 @@
         <v>2.7116703072703601</v>
       </c>
       <c r="C34">
-        <v>2.7117607798029</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7112775894740602</v>
+      </c>
+      <c r="X34">
+        <v>33</v>
+      </c>
+      <c r="Y34">
+        <v>0.81246801191321905</v>
+      </c>
+      <c r="Z34">
+        <v>4230.3187759682496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2.96999999999999</v>
       </c>
@@ -10647,10 +13118,10 @@
         <v>2.7575321893981899</v>
       </c>
       <c r="C35">
-        <v>2.7577921599366602</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7576774673033602</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3.0599999999999898</v>
       </c>
@@ -10658,10 +13129,10 @@
         <v>2.8023659472272802</v>
       </c>
       <c r="C36">
-        <v>2.8028583100604201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.8031010092570399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3.1499999999999901</v>
       </c>
@@ -10669,10 +13140,10 @@
         <v>2.8462166684852099</v>
       </c>
       <c r="C37">
-        <v>2.8469959086985699</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.8475829235065202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3.23999999999999</v>
       </c>
@@ -10680,10 +13151,10 @@
         <v>2.88912653848773</v>
       </c>
       <c r="C38">
-        <v>2.8902394511536902</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.89115578522195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3.3299999999999899</v>
       </c>
@@ -10691,10 +13162,10 @@
         <v>2.93113508402879</v>
       </c>
       <c r="C39">
-        <v>2.9326212985389799</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.93385026577034</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3.4199999999999902</v>
       </c>
@@ -10702,10 +13173,10 @@
         <v>2.9722793921792099</v>
       </c>
       <c r="C40">
-        <v>2.9741720397290199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.9756953272858002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3.50999999999999</v>
       </c>
@@ -10713,10 +13184,10 @@
         <v>3.0125943070291701</v>
       </c>
       <c r="C41">
-        <v>3.0149205078523398</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0167183886662001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3.5999999999999899</v>
       </c>
@@ -10724,10 +13195,10 @@
         <v>3.0521126069900899</v>
       </c>
       <c r="C42">
-        <v>3.0548939062376901</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0569454679245398</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3.6899999999999902</v>
       </c>
@@ -10735,10 +13206,10 @@
         <v>3.0908651649163699</v>
       </c>
       <c r="C43">
-        <v>3.0941180840304998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.09640130491234</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3.77999999999999</v>
       </c>
@@ -10746,10 +13217,10 @@
         <v>3.1288810930067199</v>
       </c>
       <c r="C44">
-        <v>3.13261741362225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.13510946769577</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3.8699999999999899</v>
       </c>
@@ -10757,10 +13228,10 @@
         <v>3.1661878741889899</v>
       </c>
       <c r="C45">
-        <v>3.17041504185765</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.17309244526886</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3.9599999999999902</v>
       </c>
@@ -10768,10 +13239,10 @@
         <v>3.2028114814736699</v>
       </c>
       <c r="C46">
-        <v>3.2075329417465599</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.2103717288048301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4.0499999999999901</v>
       </c>
@@ -10779,10 +13250,10 @@
         <v>3.2387764865745301</v>
       </c>
       <c r="C47">
-        <v>3.2439919939635198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.2469678832543898</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4.1399999999999899</v>
       </c>
@@ -10790,7 +13261,7 @@
         <v>3.2741061589341398</v>
       </c>
       <c r="C48">
-        <v>3.2798120611694701</v>
+        <v>3.2829006107813599</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -10801,7 +13272,7 @@
         <v>3.3088225561536602</v>
       </c>
       <c r="C49">
-        <v>3.3150120559033698</v>
+        <v>3.3181888072664401</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -10812,7 +13283,7 @@
         <v>3.3429466067071001</v>
       </c>
       <c r="C50">
-        <v>3.3496100027028399</v>
+        <v>3.3528506128986999</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -10823,7 +13294,7 @@
         <v>3.3764981857167702</v>
       </c>
       <c r="C51">
-        <v>3.3836230950364001</v>
+        <v>3.3869034577016102</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -10834,7 +13305,7 @@
         <v>3.4094961844768399</v>
       </c>
       <c r="C52">
-        <v>3.4170677475639901</v>
+        <v>3.42036410269897</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -10845,7 +13316,7 @@
         <v>3.4419585743340102</v>
       </c>
       <c r="C53">
-        <v>3.4499596441862801</v>
+        <v>3.4532486773103099</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -10856,7 +13327,7 @@
         <v>3.4739024654661099</v>
       </c>
       <c r="C54">
-        <v>3.48231378229648</v>
+        <v>3.4855727134699701</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -10867,7 +13338,7 @@
         <v>3.5053441610400098</v>
       </c>
       <c r="C55">
-        <v>3.5141445136127798</v>
+        <v>3.5173511768856098</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -10878,7 +13349,7 @@
         <v>3.5362992071778399</v>
       </c>
       <c r="C56">
-        <v>3.5454655819511198</v>
+        <v>3.5485984957870702</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -10889,7 +13360,7 @@
         <v>3.56678243911507</v>
       </c>
       <c r="C57">
-        <v>3.5762901583148601</v>
+        <v>3.5793285874628</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -10900,7 +13371,7 @@
         <v>3.5968080238934399</v>
       </c>
       <c r="C58">
-        <v>3.6066308737891499</v>
+        <v>3.6095548828367701</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -10911,7 +13382,7 @@
         <v>3.6263894998962298</v>
       </c>
       <c r="C59">
-        <v>3.6364998511558899</v>
+        <v>3.6392903493014699</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -10922,7 +13393,7 @@
         <v>3.6555398135021702</v>
       </c>
       <c r="C60">
-        <v>3.6659087379020798</v>
+        <v>3.6685475119919202</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -10933,7 +13404,7 @@
         <v>3.6842713531062401</v>
       </c>
       <c r="C61">
-        <v>3.69486875274885</v>
+        <v>3.69733847365982</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -10944,7 +13415,7 @@
         <v>3.7125959807312499</v>
       </c>
       <c r="C62">
-        <v>3.7233908460263301</v>
+        <v>3.7256749332851</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -10955,7 +13426,7 @@
         <v>3.74052506143199</v>
       </c>
       <c r="C63">
-        <v>3.75149572672274</v>
+        <v>3.75356820354409</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -10966,7 +13437,7 @@
         <v>3.7680694906744501</v>
       </c>
       <c r="C64">
-        <v>3.7791584246191099</v>
+        <v>3.7810292272381498</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -10977,7 +13448,7 @@
         <v>3.79523971985506</v>
       </c>
       <c r="C65">
-        <v>3.80642643116418</v>
+        <v>3.80806859277356</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -10988,7 +13459,7 @@
         <v>3.8220457801097401</v>
       </c>
       <c r="C66">
-        <v>3.8332948728413698</v>
+        <v>3.8346965487723099</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -10999,7 +13470,7 @@
         <v>3.84849730454826</v>
       </c>
       <c r="C67">
-        <v>3.8597729189286198</v>
+        <v>3.8609230178843701</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -11010,7 +13481,7 @@
         <v>3.87460354903742</v>
       </c>
       <c r="C68">
-        <v>3.8858691739590299</v>
+        <v>3.8867576098635599</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -11021,7 +13492,7 @@
         <v>3.9003734116451398</v>
       </c>
       <c r="C69">
-        <v>3.9115918975339201</v>
+        <v>3.91220963396258</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -11032,7 +13503,7 @@
         <v>3.9258154508477601</v>
       </c>
       <c r="C70">
-        <v>3.9369490452361302</v>
+        <v>3.9372881106967301</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -11043,7 +13514,7 @@
         <v>3.9509379025937101</v>
       </c>
       <c r="C71">
-        <v>3.9619482880564498</v>
+        <v>3.96200178302059</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -11054,7 +13525,7 @@
         <v>3.9757486963086799</v>
       </c>
       <c r="C72">
-        <v>3.9865970265755801</v>
+        <v>3.9863591269578298</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -11065,7 +13536,7 @@
         <v>4.0002554699202104</v>
       </c>
       <c r="C73">
-        <v>4.0109024030858498</v>
+        <v>4.0103683617200998</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -11076,7 +13547,7 @@
         <v>4.0244655839727699</v>
       </c>
       <c r="C74">
-        <v>4.0348713125397104</v>
+        <v>4.0340374593478296</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -11087,7 +13558,7 @@
         <v>4.0483861348987098</v>
       </c>
       <c r="C75">
-        <v>4.0585104126464397</v>
+        <v>4.0573741539027299</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -11098,7 +13569,7 @@
         <v>4.0720239675049896</v>
       </c>
       <c r="C76">
-        <v>4.08182613326428</v>
+        <v>4.08038595023912</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -11109,7 +13580,7 @@
         <v>4.0953856867305101</v>
       </c>
       <c r="C77">
-        <v>4.1048246851713097</v>
+        <v>4.1030801323792199</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -11120,7 +13591,7 @@
         <v>4.1184776687246298</v>
       </c>
       <c r="C78">
-        <v>4.1275120682709998</v>
+        <v>4.1254637715149798</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -11131,7 +13602,7 @@
         <v>4.1413060712935099</v>
       </c>
       <c r="C79">
-        <v>4.1498940792749401</v>
+        <v>4.1475437336578196</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -11142,7 +13613,7 @@
         <v>4.1638768437568396</v>
       </c>
       <c r="C80">
-        <v>4.17197631889759</v>
+        <v>4.1693266869555803</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -11153,7 +13624,7 @@
         <v>4.18619573625464</v>
       </c>
       <c r="C81">
-        <v>4.1937641985925502</v>
+        <v>4.1908191086947797</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -11164,7 +13635,7 @@
         <v>4.2082683085404096</v>
       </c>
       <c r="C82">
-        <v>4.2152629468563703</v>
+        <v>4.21202729200491</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -11175,7 +13646,7 @@
         <v>4.2300999382943996</v>
       </c>
       <c r="C83">
-        <v>4.2364776151227597</v>
+        <v>4.2329573522802901</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -11186,7 +13657,7 @@
         <v>4.2516958289879803</v>
       </c>
       <c r="C84">
-        <v>4.2574130832677302</v>
+        <v>4.2536152333341199</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -11197,7 +13668,7 @@
         <v>4.2730610173279198</v>
       </c>
       <c r="C85">
-        <v>4.2780740647437199</v>
+        <v>4.2740067132980304</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -11208,7 +13679,7 @@
         <v>4.2942003803072897</v>
       </c>
       <c r="C86">
-        <v>4.29846511135894</v>
+        <v>4.2941374102801202</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -11219,7 +13690,7 @@
         <v>4.3151186418875698</v>
       </c>
       <c r="C87">
-        <v>4.3185906177162501</v>
+        <v>4.3140127877930601</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -11230,7 +13701,7 @@
         <v>4.33582037933488</v>
       </c>
       <c r="C88">
-        <v>4.3384548253241499</v>
+        <v>4.3336381599635798</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -11241,7 +13712,7 @@
         <v>4.3563100292317296</v>
       </c>
       <c r="C89">
-        <v>4.3580618263907898</v>
+        <v>4.3530186965337601</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -11252,7 +13723,7 @@
         <v>4.3765918931838304</v>
       </c>
       <c r="C90">
-        <v>4.3774155673103303</v>
+        <v>4.3721594276639504</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -11263,7 +13734,7 @@
         <v>4.39667014324049</v>
       </c>
       <c r="C91">
-        <v>4.3965198518496198</v>
+        <v>4.3910652485466501</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -11274,7 +13745,7 @@
         <v>4.4165488270455997</v>
       </c>
       <c r="C92">
-        <v>4.4153783440413603</v>
+        <v>4.4097409238400296</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -11285,7 +13756,7 @@
         <v>4.4362318727351902</v>
       </c>
       <c r="C93">
-        <v>4.43399457078878</v>
+        <v>4.4281910919294001</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -11296,7 +13767,7 @@
         <v>4.4557230935962098</v>
       </c>
       <c r="C94">
-        <v>4.45237192418523</v>
+        <v>4.4464202690244896</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -11307,7 +13778,7 @@
         <v>4.4750261925006596</v>
       </c>
       <c r="C95">
-        <v>4.4705136635506699</v>
+        <v>4.4644328530997504</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -11318,7 +13789,7 @@
         <v>4.4941447661275697</v>
       </c>
       <c r="C96">
-        <v>4.4884229171855603</v>
+        <v>4.4822331276848804</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -11329,7 +13800,7 @@
         <v>4.5130823089852701</v>
       </c>
       <c r="C97">
-        <v>4.5061026838412097</v>
+        <v>4.4998252655120297</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -11340,7 +13811,7 @@
         <v>4.5318422172449004</v>
       </c>
       <c r="C98">
-        <v>4.5235558339039201</v>
+        <v>4.5172133320260501</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -11351,7 +13822,7 @@
         <v>4.5504277923958201</v>
       </c>
       <c r="C99">
-        <v>4.5407851102889003</v>
+        <v>4.5344012887637497</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -11362,7 +13833,7 @@
         <v>4.5688422447327399</v>
       </c>
       <c r="C100">
-        <v>4.5577931290379397</v>
+        <v>4.5513929966077598</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -11373,7 +13844,7 @@
         <v>4.5870886966837903</v>
       </c>
       <c r="C101">
-        <v>4.5745823796132603</v>
+        <v>4.5681922189203501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>